<commit_message>
Fixed an issue in which there was a silent error if 'choices' or 'external_choices' worksheets had no header row.
</commit_message>
<xml_diff>
--- a/test/files/multiple_file_language_option_conversion/BFR5-Household-Questionnaire-v13-jef.xlsx
+++ b/test/files/multiple_file_language_option_conversion/BFR5-Household-Questionnaire-v13-jef.xlsx
@@ -5162,9 +5162,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5507,1007 +5514,1007 @@
   </borders>
   <cellStyleXfs count="1000">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6521,40 +6528,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="126"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="126"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6569,7 +6576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6584,10 +6591,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6606,52 +6613,52 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6660,7 +6667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6669,10 +6676,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6687,34 +6694,34 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="487"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="487" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="487"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="487" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6727,7 +6734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6737,17 +6744,17 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -6757,7 +6764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6771,68 +6778,69 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="487" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1000">
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
@@ -8137,10 +8145,10 @@
   <dimension ref="A1:IX376"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P63" sqref="P63"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -21626,7 +21634,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21640,7 +21648,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="75"/>
+      <c r="A1" s="130"/>
       <c r="B1" s="75"/>
       <c r="C1" s="75"/>
       <c r="D1" s="76"/>

</xml_diff>